<commit_message>
Add Vmpp, Impp, FF, Grade and recurrence columns
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="measured_current">Sheet1!$A:$A</definedName>
   </definedNames>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -1782,32 +1782,32 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T46"/>
+  <dimension ref="A1:Y47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
     <col width="14.77734375" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="13.5546875" customWidth="1" min="3" max="4"/>
-    <col width="14" customWidth="1" min="5" max="5"/>
-    <col width="14.21875" customWidth="1" min="6" max="6"/>
-    <col width="22.77734375" customWidth="1" min="7" max="7"/>
-    <col width="21.44140625" customWidth="1" min="8" max="8"/>
-    <col width="18.33203125" customWidth="1" min="9" max="9"/>
-    <col width="17.5546875" customWidth="1" min="10" max="10"/>
-    <col width="16.5546875" customWidth="1" min="11" max="11"/>
-    <col width="15.5546875" customWidth="1" min="12" max="12"/>
-    <col width="15.21875" customWidth="1" min="13" max="13"/>
-    <col width="16.33203125" customWidth="1" min="14" max="14"/>
-    <col width="29.44140625" customWidth="1" min="15" max="15"/>
-    <col width="26.88671875" customWidth="1" min="16" max="16"/>
-    <col width="18.109375" customWidth="1" min="17" max="17"/>
-    <col width="14" customWidth="1" min="18" max="18"/>
-    <col width="12.44140625" customWidth="1" min="19" max="19"/>
-    <col width="15.109375" customWidth="1" min="20" max="20"/>
+    <col width="13.5546875" customWidth="1" min="3" max="6"/>
+    <col width="14" customWidth="1" min="7" max="7"/>
+    <col width="14.21875" customWidth="1" min="8" max="11"/>
+    <col width="22.77734375" customWidth="1" min="12" max="12"/>
+    <col width="21.44140625" customWidth="1" min="13" max="13"/>
+    <col width="18.33203125" customWidth="1" min="14" max="14"/>
+    <col width="17.5546875" customWidth="1" min="15" max="15"/>
+    <col width="16.5546875" customWidth="1" min="16" max="16"/>
+    <col width="15.5546875" customWidth="1" min="17" max="17"/>
+    <col width="15.21875" customWidth="1" min="18" max="18"/>
+    <col width="16.33203125" customWidth="1" min="19" max="19"/>
+    <col width="29.44140625" customWidth="1" min="20" max="20"/>
+    <col width="26.88671875" customWidth="1" min="21" max="21"/>
+    <col width="18.109375" customWidth="1" min="22" max="22"/>
+    <col width="14" customWidth="1" min="23" max="23"/>
+    <col width="12.44140625" customWidth="1" min="24" max="24"/>
+    <col width="15.109375" customWidth="1" min="25" max="25"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1819,6 +1819,8 @@
       <c r="B1" s="1" t="n"/>
       <c r="D1" s="2" t="n"/>
       <c r="E1" s="2" t="n"/>
+      <c r="F1" s="2" t="n"/>
+      <c r="G1" s="2" t="n"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -1843,80 +1845,105 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
+          <t>Imp</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Vmp</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
           <t>Uoc</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>Isc</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>FF</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Grade</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Recurrence</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
         <is>
           <t>Temperature Ambient</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="M2" t="inlineStr">
         <is>
           <t>Temperature Lamps</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="N2" t="inlineStr">
         <is>
           <t>Pmpp Reference</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="O2" t="inlineStr">
         <is>
           <t>Pmpp Deviation</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="P2" t="inlineStr">
         <is>
           <t>Uoc Reference</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="Q2" t="inlineStr">
         <is>
           <t>Uoc Deviation</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="R2" t="inlineStr">
         <is>
           <t>Isc Reference</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
+      <c r="S2" t="inlineStr">
         <is>
           <t>Isc Deviation</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr">
+      <c r="T2" t="inlineStr">
         <is>
           <t>Temperature Ambient Reference</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
+      <c r="U2" t="inlineStr">
         <is>
           <t>Temperature Lamps Reference</t>
         </is>
       </c>
-      <c r="Q2" t="inlineStr">
+      <c r="V2" t="inlineStr">
         <is>
           <t>Reference Number</t>
         </is>
       </c>
-      <c r="R2" t="inlineStr">
+      <c r="W2" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="S2" t="inlineStr">
+      <c r="X2" t="inlineStr">
         <is>
           <t>Time</t>
         </is>
       </c>
-      <c r="T2" t="inlineStr">
+      <c r="Y2" t="inlineStr">
         <is>
           <t>Serial Number</t>
         </is>
@@ -1935,56 +1962,56 @@
       <c r="D3" t="n">
         <v>0</v>
       </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0</v>
-      </c>
       <c r="G3" t="n">
         <v>0</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
       </c>
-      <c r="I3" t="n">
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" t="n">
         <v>31.0654</v>
       </c>
-      <c r="J3" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" t="n">
+      <c r="O3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P3" t="n">
         <v>9.933199999999999</v>
       </c>
-      <c r="L3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M3" t="n">
+      <c r="Q3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" t="n">
         <v>4.3456</v>
       </c>
-      <c r="N3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P3" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>0</v>
-      </c>
-      <c r="R3" t="inlineStr">
+      <c r="S3" t="n">
+        <v>0</v>
+      </c>
+      <c r="T3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U3" t="n">
+        <v>2</v>
+      </c>
+      <c r="V3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W3" t="inlineStr">
         <is>
           <t>07/18/2024</t>
         </is>
       </c>
-      <c r="S3" t="inlineStr">
+      <c r="X3" t="inlineStr">
         <is>
           <t>13:46:06</t>
         </is>
       </c>
-      <c r="T3" t="inlineStr">
+      <c r="Y3" t="inlineStr">
         <is>
           <t>00000001</t>
         </is>
@@ -2003,56 +2030,56 @@
       <c r="D4" t="n">
         <v>0</v>
       </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
       <c r="G4" t="n">
         <v>0</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
       </c>
-      <c r="I4" t="n">
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" t="n">
         <v>31.0654</v>
       </c>
-      <c r="J4" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" t="n">
+      <c r="O4" t="n">
+        <v>0</v>
+      </c>
+      <c r="P4" t="n">
         <v>9.933199999999999</v>
       </c>
-      <c r="L4" t="n">
-        <v>0</v>
-      </c>
-      <c r="M4" t="n">
+      <c r="Q4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" t="n">
         <v>4.3456</v>
       </c>
-      <c r="N4" t="n">
-        <v>0</v>
-      </c>
-      <c r="O4" t="n">
-        <v>0</v>
-      </c>
-      <c r="P4" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R4" t="inlineStr">
+      <c r="S4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0</v>
+      </c>
+      <c r="U4" t="n">
+        <v>2</v>
+      </c>
+      <c r="V4" t="n">
+        <v>0</v>
+      </c>
+      <c r="W4" t="inlineStr">
         <is>
           <t>07/18/2024</t>
         </is>
       </c>
-      <c r="S4" t="inlineStr">
+      <c r="X4" t="inlineStr">
         <is>
           <t>13:46:44</t>
         </is>
       </c>
-      <c r="T4" t="inlineStr">
+      <c r="Y4" t="inlineStr">
         <is>
           <t>00000001</t>
         </is>
@@ -2071,56 +2098,56 @@
       <c r="D5" t="n">
         <v>0</v>
       </c>
-      <c r="E5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0</v>
-      </c>
       <c r="G5" t="n">
         <v>0</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
       </c>
-      <c r="I5" t="n">
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="n">
         <v>31.0654</v>
       </c>
-      <c r="J5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" t="n">
+      <c r="O5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" t="n">
         <v>9.933199999999999</v>
       </c>
-      <c r="L5" t="n">
-        <v>0</v>
-      </c>
-      <c r="M5" t="n">
+      <c r="Q5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R5" t="n">
         <v>4.3456</v>
       </c>
-      <c r="N5" t="n">
-        <v>0</v>
-      </c>
-      <c r="O5" t="n">
-        <v>0</v>
-      </c>
-      <c r="P5" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>0</v>
-      </c>
-      <c r="R5" t="inlineStr">
+      <c r="S5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0</v>
+      </c>
+      <c r="U5" t="n">
+        <v>2</v>
+      </c>
+      <c r="V5" t="n">
+        <v>0</v>
+      </c>
+      <c r="W5" t="inlineStr">
         <is>
           <t>07/18/2024</t>
         </is>
       </c>
-      <c r="S5" t="inlineStr">
+      <c r="X5" t="inlineStr">
         <is>
           <t>13:48:15</t>
         </is>
       </c>
-      <c r="T5" t="inlineStr">
+      <c r="Y5" t="inlineStr">
         <is>
           <t>00000001</t>
         </is>
@@ -2139,51 +2166,51 @@
       <c r="D6" t="n">
         <v>0</v>
       </c>
-      <c r="E6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0</v>
-      </c>
       <c r="G6" t="n">
         <v>0</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
       </c>
-      <c r="I6" t="n">
+      <c r="L6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" t="n">
         <v>31.0654</v>
       </c>
-      <c r="J6" t="n">
-        <v>0</v>
-      </c>
-      <c r="K6" t="n">
+      <c r="O6" t="n">
+        <v>0</v>
+      </c>
+      <c r="P6" t="n">
         <v>9.933199999999999</v>
       </c>
-      <c r="L6" t="n">
-        <v>0</v>
-      </c>
-      <c r="M6" t="n">
+      <c r="Q6" t="n">
+        <v>0</v>
+      </c>
+      <c r="R6" t="n">
         <v>4.3456</v>
       </c>
-      <c r="N6" t="n">
-        <v>0</v>
-      </c>
-      <c r="O6" t="n">
-        <v>0</v>
-      </c>
-      <c r="P6" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>0</v>
-      </c>
-      <c r="R6" t="inlineStr">
+      <c r="S6" t="n">
+        <v>0</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0</v>
+      </c>
+      <c r="U6" t="n">
+        <v>2</v>
+      </c>
+      <c r="V6" t="n">
+        <v>0</v>
+      </c>
+      <c r="W6" t="inlineStr">
         <is>
           <t>07/22/2024</t>
         </is>
       </c>
-      <c r="S6" t="inlineStr">
+      <c r="X6" t="inlineStr">
         <is>
           <t>09:59:04</t>
         </is>
@@ -2202,56 +2229,56 @@
       <c r="D7" t="n">
         <v>0</v>
       </c>
-      <c r="E7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0</v>
-      </c>
       <c r="G7" t="n">
         <v>0</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
       </c>
-      <c r="I7" t="n">
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" t="n">
         <v>31.0654</v>
       </c>
-      <c r="J7" t="n">
-        <v>0</v>
-      </c>
-      <c r="K7" t="n">
+      <c r="O7" t="n">
+        <v>0</v>
+      </c>
+      <c r="P7" t="n">
         <v>9.933199999999999</v>
       </c>
-      <c r="L7" t="n">
-        <v>0</v>
-      </c>
-      <c r="M7" t="n">
+      <c r="Q7" t="n">
+        <v>0</v>
+      </c>
+      <c r="R7" t="n">
         <v>4.3456</v>
       </c>
-      <c r="N7" t="n">
-        <v>0</v>
-      </c>
-      <c r="O7" t="n">
-        <v>0</v>
-      </c>
-      <c r="P7" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q7" t="n">
-        <v>0</v>
-      </c>
-      <c r="R7" t="inlineStr">
+      <c r="S7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0</v>
+      </c>
+      <c r="U7" t="n">
+        <v>2</v>
+      </c>
+      <c r="V7" t="n">
+        <v>0</v>
+      </c>
+      <c r="W7" t="inlineStr">
         <is>
           <t>07/24/2024</t>
         </is>
       </c>
-      <c r="S7" t="inlineStr">
+      <c r="X7" t="inlineStr">
         <is>
           <t>11:01:38</t>
         </is>
       </c>
-      <c r="T7" t="inlineStr">
+      <c r="Y7" t="inlineStr">
         <is>
           <t>02314352</t>
         </is>
@@ -2270,56 +2297,56 @@
       <c r="D8" t="n">
         <v>0</v>
       </c>
-      <c r="E8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0</v>
-      </c>
       <c r="G8" t="n">
         <v>0</v>
       </c>
       <c r="H8" t="n">
         <v>0</v>
       </c>
-      <c r="I8" t="n">
+      <c r="L8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" t="n">
         <v>31.0654</v>
       </c>
-      <c r="J8" t="n">
-        <v>0</v>
-      </c>
-      <c r="K8" t="n">
+      <c r="O8" t="n">
+        <v>0</v>
+      </c>
+      <c r="P8" t="n">
         <v>9.933199999999999</v>
       </c>
-      <c r="L8" t="n">
-        <v>0</v>
-      </c>
-      <c r="M8" t="n">
+      <c r="Q8" t="n">
+        <v>0</v>
+      </c>
+      <c r="R8" t="n">
         <v>4.3456</v>
       </c>
-      <c r="N8" t="n">
-        <v>0</v>
-      </c>
-      <c r="O8" t="n">
-        <v>0</v>
-      </c>
-      <c r="P8" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q8" t="n">
-        <v>0</v>
-      </c>
-      <c r="R8" t="inlineStr">
+      <c r="S8" t="n">
+        <v>0</v>
+      </c>
+      <c r="T8" t="n">
+        <v>0</v>
+      </c>
+      <c r="U8" t="n">
+        <v>2</v>
+      </c>
+      <c r="V8" t="n">
+        <v>0</v>
+      </c>
+      <c r="W8" t="inlineStr">
         <is>
           <t>07/24/2024</t>
         </is>
       </c>
-      <c r="S8" t="inlineStr">
+      <c r="X8" t="inlineStr">
         <is>
           <t>11:02:41</t>
         </is>
       </c>
-      <c r="T8" t="inlineStr">
+      <c r="Y8" t="inlineStr">
         <is>
           <t>0231435234</t>
         </is>
@@ -2338,51 +2365,51 @@
       <c r="D9" t="n">
         <v>0</v>
       </c>
-      <c r="E9" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0</v>
-      </c>
       <c r="G9" t="n">
         <v>0</v>
       </c>
       <c r="H9" t="n">
         <v>0</v>
       </c>
-      <c r="I9" t="n">
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" t="n">
         <v>31.0654</v>
       </c>
-      <c r="J9" t="n">
-        <v>0</v>
-      </c>
-      <c r="K9" t="n">
+      <c r="O9" t="n">
+        <v>0</v>
+      </c>
+      <c r="P9" t="n">
         <v>9.933199999999999</v>
       </c>
-      <c r="L9" t="n">
-        <v>0</v>
-      </c>
-      <c r="M9" t="n">
+      <c r="Q9" t="n">
+        <v>0</v>
+      </c>
+      <c r="R9" t="n">
         <v>4.3456</v>
       </c>
-      <c r="N9" t="n">
-        <v>0</v>
-      </c>
-      <c r="O9" t="n">
-        <v>0</v>
-      </c>
-      <c r="P9" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q9" t="n">
-        <v>0</v>
-      </c>
-      <c r="R9" t="inlineStr">
+      <c r="S9" t="n">
+        <v>0</v>
+      </c>
+      <c r="T9" t="n">
+        <v>0</v>
+      </c>
+      <c r="U9" t="n">
+        <v>2</v>
+      </c>
+      <c r="V9" t="n">
+        <v>0</v>
+      </c>
+      <c r="W9" t="inlineStr">
         <is>
           <t>07/24/2024</t>
         </is>
       </c>
-      <c r="S9" t="inlineStr">
+      <c r="X9" t="inlineStr">
         <is>
           <t>12:12:14</t>
         </is>
@@ -2401,51 +2428,51 @@
       <c r="D10" t="n">
         <v>0</v>
       </c>
-      <c r="E10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0</v>
-      </c>
       <c r="G10" t="n">
         <v>0</v>
       </c>
       <c r="H10" t="n">
         <v>0</v>
       </c>
-      <c r="I10" t="n">
+      <c r="L10" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" t="n">
         <v>31.0654</v>
       </c>
-      <c r="J10" t="n">
-        <v>0</v>
-      </c>
-      <c r="K10" t="n">
+      <c r="O10" t="n">
+        <v>0</v>
+      </c>
+      <c r="P10" t="n">
         <v>9.933199999999999</v>
       </c>
-      <c r="L10" t="n">
-        <v>0</v>
-      </c>
-      <c r="M10" t="n">
+      <c r="Q10" t="n">
+        <v>0</v>
+      </c>
+      <c r="R10" t="n">
         <v>4.3456</v>
       </c>
-      <c r="N10" t="n">
-        <v>0</v>
-      </c>
-      <c r="O10" t="n">
-        <v>0</v>
-      </c>
-      <c r="P10" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q10" t="n">
-        <v>0</v>
-      </c>
-      <c r="R10" t="inlineStr">
+      <c r="S10" t="n">
+        <v>0</v>
+      </c>
+      <c r="T10" t="n">
+        <v>0</v>
+      </c>
+      <c r="U10" t="n">
+        <v>2</v>
+      </c>
+      <c r="V10" t="n">
+        <v>0</v>
+      </c>
+      <c r="W10" t="inlineStr">
         <is>
           <t>07/24/2024</t>
         </is>
       </c>
-      <c r="S10" t="inlineStr">
+      <c r="X10" t="inlineStr">
         <is>
           <t>15:27:15</t>
         </is>
@@ -2464,56 +2491,56 @@
       <c r="D11" t="n">
         <v>0</v>
       </c>
-      <c r="E11" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0</v>
-      </c>
       <c r="G11" t="n">
         <v>0</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
       </c>
-      <c r="I11" t="n">
+      <c r="L11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0</v>
+      </c>
+      <c r="N11" t="n">
         <v>31.0654</v>
       </c>
-      <c r="J11" t="n">
-        <v>0</v>
-      </c>
-      <c r="K11" t="n">
+      <c r="O11" t="n">
+        <v>0</v>
+      </c>
+      <c r="P11" t="n">
         <v>9.933199999999999</v>
       </c>
-      <c r="L11" t="n">
-        <v>0</v>
-      </c>
-      <c r="M11" t="n">
+      <c r="Q11" t="n">
+        <v>0</v>
+      </c>
+      <c r="R11" t="n">
         <v>4.3456</v>
       </c>
-      <c r="N11" t="n">
-        <v>0</v>
-      </c>
-      <c r="O11" t="n">
-        <v>0</v>
-      </c>
-      <c r="P11" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q11" t="n">
-        <v>0</v>
-      </c>
-      <c r="R11" t="inlineStr">
+      <c r="S11" t="n">
+        <v>0</v>
+      </c>
+      <c r="T11" t="n">
+        <v>0</v>
+      </c>
+      <c r="U11" t="n">
+        <v>2</v>
+      </c>
+      <c r="V11" t="n">
+        <v>0</v>
+      </c>
+      <c r="W11" t="inlineStr">
         <is>
           <t>07/24/2024</t>
         </is>
       </c>
-      <c r="S11" t="inlineStr">
+      <c r="X11" t="inlineStr">
         <is>
           <t>15:28:03</t>
         </is>
       </c>
-      <c r="T11" t="inlineStr">
+      <c r="Y11" t="inlineStr">
         <is>
           <t>00000003</t>
         </is>
@@ -2532,51 +2559,51 @@
       <c r="D12" t="n">
         <v>0</v>
       </c>
-      <c r="E12" t="n">
-        <v>0</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0</v>
-      </c>
       <c r="G12" t="n">
         <v>0</v>
       </c>
       <c r="H12" t="n">
         <v>0</v>
       </c>
-      <c r="I12" t="n">
+      <c r="L12" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" t="n">
         <v>31.0654</v>
       </c>
-      <c r="J12" t="n">
-        <v>0</v>
-      </c>
-      <c r="K12" t="n">
+      <c r="O12" t="n">
+        <v>0</v>
+      </c>
+      <c r="P12" t="n">
         <v>9.933199999999999</v>
       </c>
-      <c r="L12" t="n">
-        <v>0</v>
-      </c>
-      <c r="M12" t="n">
+      <c r="Q12" t="n">
+        <v>0</v>
+      </c>
+      <c r="R12" t="n">
         <v>4.3456</v>
       </c>
-      <c r="N12" t="n">
-        <v>0</v>
-      </c>
-      <c r="O12" t="n">
-        <v>0</v>
-      </c>
-      <c r="P12" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q12" t="n">
-        <v>0</v>
-      </c>
-      <c r="R12" t="inlineStr">
+      <c r="S12" t="n">
+        <v>0</v>
+      </c>
+      <c r="T12" t="n">
+        <v>0</v>
+      </c>
+      <c r="U12" t="n">
+        <v>2</v>
+      </c>
+      <c r="V12" t="n">
+        <v>0</v>
+      </c>
+      <c r="W12" t="inlineStr">
         <is>
           <t>07/24/2024</t>
         </is>
       </c>
-      <c r="S12" t="inlineStr">
+      <c r="X12" t="inlineStr">
         <is>
           <t>15:59:36</t>
         </is>
@@ -2595,51 +2622,51 @@
       <c r="D13" t="n">
         <v>0</v>
       </c>
-      <c r="E13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F13" t="n">
-        <v>0</v>
-      </c>
       <c r="G13" t="n">
         <v>0</v>
       </c>
       <c r="H13" t="n">
         <v>0</v>
       </c>
-      <c r="I13" t="n">
+      <c r="L13" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" t="n">
         <v>31.0654</v>
       </c>
-      <c r="J13" t="n">
-        <v>0</v>
-      </c>
-      <c r="K13" t="n">
+      <c r="O13" t="n">
+        <v>0</v>
+      </c>
+      <c r="P13" t="n">
         <v>9.933199999999999</v>
       </c>
-      <c r="L13" t="n">
-        <v>0</v>
-      </c>
-      <c r="M13" t="n">
+      <c r="Q13" t="n">
+        <v>0</v>
+      </c>
+      <c r="R13" t="n">
         <v>4.3456</v>
       </c>
-      <c r="N13" t="n">
-        <v>0</v>
-      </c>
-      <c r="O13" t="n">
-        <v>0</v>
-      </c>
-      <c r="P13" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q13" t="n">
-        <v>0</v>
-      </c>
-      <c r="R13" t="inlineStr">
+      <c r="S13" t="n">
+        <v>0</v>
+      </c>
+      <c r="T13" t="n">
+        <v>0</v>
+      </c>
+      <c r="U13" t="n">
+        <v>2</v>
+      </c>
+      <c r="V13" t="n">
+        <v>0</v>
+      </c>
+      <c r="W13" t="inlineStr">
         <is>
           <t>07/24/2024</t>
         </is>
       </c>
-      <c r="S13" t="inlineStr">
+      <c r="X13" t="inlineStr">
         <is>
           <t>16:16:18</t>
         </is>
@@ -2658,51 +2685,51 @@
       <c r="D14" t="n">
         <v>0</v>
       </c>
-      <c r="E14" t="n">
-        <v>0</v>
-      </c>
-      <c r="F14" t="n">
-        <v>0</v>
-      </c>
       <c r="G14" t="n">
         <v>0</v>
       </c>
       <c r="H14" t="n">
         <v>0</v>
       </c>
-      <c r="I14" t="n">
+      <c r="L14" t="n">
+        <v>0</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0</v>
+      </c>
+      <c r="N14" t="n">
         <v>31.0654</v>
       </c>
-      <c r="J14" t="n">
-        <v>0</v>
-      </c>
-      <c r="K14" t="n">
+      <c r="O14" t="n">
+        <v>0</v>
+      </c>
+      <c r="P14" t="n">
         <v>9.933199999999999</v>
       </c>
-      <c r="L14" t="n">
-        <v>0</v>
-      </c>
-      <c r="M14" t="n">
+      <c r="Q14" t="n">
+        <v>0</v>
+      </c>
+      <c r="R14" t="n">
         <v>4.3456</v>
       </c>
-      <c r="N14" t="n">
-        <v>0</v>
-      </c>
-      <c r="O14" t="n">
-        <v>0</v>
-      </c>
-      <c r="P14" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q14" t="n">
-        <v>0</v>
-      </c>
-      <c r="R14" t="inlineStr">
+      <c r="S14" t="n">
+        <v>0</v>
+      </c>
+      <c r="T14" t="n">
+        <v>0</v>
+      </c>
+      <c r="U14" t="n">
+        <v>2</v>
+      </c>
+      <c r="V14" t="n">
+        <v>0</v>
+      </c>
+      <c r="W14" t="inlineStr">
         <is>
           <t>07/24/2024</t>
         </is>
       </c>
-      <c r="S14" t="inlineStr">
+      <c r="X14" t="inlineStr">
         <is>
           <t>16:20:53</t>
         </is>
@@ -2721,51 +2748,51 @@
       <c r="D15" t="n">
         <v>0</v>
       </c>
-      <c r="E15" t="n">
-        <v>0</v>
-      </c>
-      <c r="F15" t="n">
-        <v>0</v>
-      </c>
       <c r="G15" t="n">
         <v>0</v>
       </c>
       <c r="H15" t="n">
         <v>0</v>
       </c>
-      <c r="I15" t="n">
+      <c r="L15" t="n">
+        <v>0</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0</v>
+      </c>
+      <c r="N15" t="n">
         <v>31.0654</v>
       </c>
-      <c r="J15" t="n">
-        <v>0</v>
-      </c>
-      <c r="K15" t="n">
+      <c r="O15" t="n">
+        <v>0</v>
+      </c>
+      <c r="P15" t="n">
         <v>9.933199999999999</v>
       </c>
-      <c r="L15" t="n">
-        <v>0</v>
-      </c>
-      <c r="M15" t="n">
+      <c r="Q15" t="n">
+        <v>0</v>
+      </c>
+      <c r="R15" t="n">
         <v>4.3456</v>
       </c>
-      <c r="N15" t="n">
-        <v>0</v>
-      </c>
-      <c r="O15" t="n">
-        <v>0</v>
-      </c>
-      <c r="P15" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q15" t="n">
-        <v>0</v>
-      </c>
-      <c r="R15" t="inlineStr">
+      <c r="S15" t="n">
+        <v>0</v>
+      </c>
+      <c r="T15" t="n">
+        <v>0</v>
+      </c>
+      <c r="U15" t="n">
+        <v>2</v>
+      </c>
+      <c r="V15" t="n">
+        <v>0</v>
+      </c>
+      <c r="W15" t="inlineStr">
         <is>
           <t>07/24/2024</t>
         </is>
       </c>
-      <c r="S15" t="inlineStr">
+      <c r="X15" t="inlineStr">
         <is>
           <t>16:21:08</t>
         </is>
@@ -2784,51 +2811,51 @@
       <c r="D16" t="n">
         <v>0</v>
       </c>
-      <c r="E16" t="n">
-        <v>0</v>
-      </c>
-      <c r="F16" t="n">
-        <v>0</v>
-      </c>
       <c r="G16" t="n">
         <v>0</v>
       </c>
       <c r="H16" t="n">
         <v>0</v>
       </c>
-      <c r="I16" t="n">
+      <c r="L16" t="n">
+        <v>0</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0</v>
+      </c>
+      <c r="N16" t="n">
         <v>31.0654</v>
       </c>
-      <c r="J16" t="n">
-        <v>0</v>
-      </c>
-      <c r="K16" t="n">
+      <c r="O16" t="n">
+        <v>0</v>
+      </c>
+      <c r="P16" t="n">
         <v>9.933199999999999</v>
       </c>
-      <c r="L16" t="n">
-        <v>0</v>
-      </c>
-      <c r="M16" t="n">
+      <c r="Q16" t="n">
+        <v>0</v>
+      </c>
+      <c r="R16" t="n">
         <v>4.3456</v>
       </c>
-      <c r="N16" t="n">
-        <v>0</v>
-      </c>
-      <c r="O16" t="n">
-        <v>0</v>
-      </c>
-      <c r="P16" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q16" t="n">
-        <v>0</v>
-      </c>
-      <c r="R16" t="inlineStr">
+      <c r="S16" t="n">
+        <v>0</v>
+      </c>
+      <c r="T16" t="n">
+        <v>0</v>
+      </c>
+      <c r="U16" t="n">
+        <v>2</v>
+      </c>
+      <c r="V16" t="n">
+        <v>0</v>
+      </c>
+      <c r="W16" t="inlineStr">
         <is>
           <t>07/24/2024</t>
         </is>
       </c>
-      <c r="S16" t="inlineStr">
+      <c r="X16" t="inlineStr">
         <is>
           <t>16:22:11</t>
         </is>
@@ -2847,51 +2874,51 @@
       <c r="D17" t="n">
         <v>0</v>
       </c>
-      <c r="E17" t="n">
-        <v>0</v>
-      </c>
-      <c r="F17" t="n">
-        <v>0</v>
-      </c>
       <c r="G17" t="n">
         <v>0</v>
       </c>
       <c r="H17" t="n">
         <v>0</v>
       </c>
-      <c r="I17" t="n">
+      <c r="L17" t="n">
+        <v>0</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0</v>
+      </c>
+      <c r="N17" t="n">
         <v>31.0654</v>
       </c>
-      <c r="J17" t="n">
-        <v>0</v>
-      </c>
-      <c r="K17" t="n">
+      <c r="O17" t="n">
+        <v>0</v>
+      </c>
+      <c r="P17" t="n">
         <v>9.933199999999999</v>
       </c>
-      <c r="L17" t="n">
-        <v>0</v>
-      </c>
-      <c r="M17" t="n">
+      <c r="Q17" t="n">
+        <v>0</v>
+      </c>
+      <c r="R17" t="n">
         <v>4.3456</v>
       </c>
-      <c r="N17" t="n">
-        <v>0</v>
-      </c>
-      <c r="O17" t="n">
-        <v>0</v>
-      </c>
-      <c r="P17" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q17" t="n">
-        <v>0</v>
-      </c>
-      <c r="R17" t="inlineStr">
+      <c r="S17" t="n">
+        <v>0</v>
+      </c>
+      <c r="T17" t="n">
+        <v>0</v>
+      </c>
+      <c r="U17" t="n">
+        <v>2</v>
+      </c>
+      <c r="V17" t="n">
+        <v>0</v>
+      </c>
+      <c r="W17" t="inlineStr">
         <is>
           <t>07/24/2024</t>
         </is>
       </c>
-      <c r="S17" t="inlineStr">
+      <c r="X17" t="inlineStr">
         <is>
           <t>16:23:52</t>
         </is>
@@ -2910,51 +2937,51 @@
       <c r="D18" t="n">
         <v>0</v>
       </c>
-      <c r="E18" t="n">
-        <v>0</v>
-      </c>
-      <c r="F18" t="n">
-        <v>0</v>
-      </c>
       <c r="G18" t="n">
         <v>0</v>
       </c>
       <c r="H18" t="n">
         <v>0</v>
       </c>
-      <c r="I18" t="n">
+      <c r="L18" t="n">
+        <v>0</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0</v>
+      </c>
+      <c r="N18" t="n">
         <v>31.0654</v>
       </c>
-      <c r="J18" t="n">
-        <v>0</v>
-      </c>
-      <c r="K18" t="n">
+      <c r="O18" t="n">
+        <v>0</v>
+      </c>
+      <c r="P18" t="n">
         <v>9.933199999999999</v>
       </c>
-      <c r="L18" t="n">
-        <v>0</v>
-      </c>
-      <c r="M18" t="n">
+      <c r="Q18" t="n">
+        <v>0</v>
+      </c>
+      <c r="R18" t="n">
         <v>4.3456</v>
       </c>
-      <c r="N18" t="n">
-        <v>0</v>
-      </c>
-      <c r="O18" t="n">
-        <v>0</v>
-      </c>
-      <c r="P18" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q18" t="n">
-        <v>0</v>
-      </c>
-      <c r="R18" t="inlineStr">
+      <c r="S18" t="n">
+        <v>0</v>
+      </c>
+      <c r="T18" t="n">
+        <v>0</v>
+      </c>
+      <c r="U18" t="n">
+        <v>2</v>
+      </c>
+      <c r="V18" t="n">
+        <v>0</v>
+      </c>
+      <c r="W18" t="inlineStr">
         <is>
           <t>07/24/2024</t>
         </is>
       </c>
-      <c r="S18" t="inlineStr">
+      <c r="X18" t="inlineStr">
         <is>
           <t>16:24:42</t>
         </is>
@@ -2973,51 +3000,51 @@
       <c r="D19" t="n">
         <v>0</v>
       </c>
-      <c r="E19" t="n">
-        <v>0</v>
-      </c>
-      <c r="F19" t="n">
-        <v>0</v>
-      </c>
       <c r="G19" t="n">
         <v>0</v>
       </c>
       <c r="H19" t="n">
         <v>0</v>
       </c>
-      <c r="I19" t="n">
+      <c r="L19" t="n">
+        <v>0</v>
+      </c>
+      <c r="M19" t="n">
+        <v>0</v>
+      </c>
+      <c r="N19" t="n">
         <v>31.0654</v>
       </c>
-      <c r="J19" t="n">
-        <v>0</v>
-      </c>
-      <c r="K19" t="n">
+      <c r="O19" t="n">
+        <v>0</v>
+      </c>
+      <c r="P19" t="n">
         <v>9.933199999999999</v>
       </c>
-      <c r="L19" t="n">
-        <v>0</v>
-      </c>
-      <c r="M19" t="n">
+      <c r="Q19" t="n">
+        <v>0</v>
+      </c>
+      <c r="R19" t="n">
         <v>4.3456</v>
       </c>
-      <c r="N19" t="n">
-        <v>0</v>
-      </c>
-      <c r="O19" t="n">
-        <v>0</v>
-      </c>
-      <c r="P19" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q19" t="n">
-        <v>0</v>
-      </c>
-      <c r="R19" t="inlineStr">
+      <c r="S19" t="n">
+        <v>0</v>
+      </c>
+      <c r="T19" t="n">
+        <v>0</v>
+      </c>
+      <c r="U19" t="n">
+        <v>2</v>
+      </c>
+      <c r="V19" t="n">
+        <v>0</v>
+      </c>
+      <c r="W19" t="inlineStr">
         <is>
           <t>07/24/2024</t>
         </is>
       </c>
-      <c r="S19" t="inlineStr">
+      <c r="X19" t="inlineStr">
         <is>
           <t>16:56:04</t>
         </is>
@@ -3036,51 +3063,51 @@
       <c r="D20" t="n">
         <v>0</v>
       </c>
-      <c r="E20" t="n">
-        <v>0</v>
-      </c>
-      <c r="F20" t="n">
-        <v>0</v>
-      </c>
       <c r="G20" t="n">
         <v>0</v>
       </c>
       <c r="H20" t="n">
         <v>0</v>
       </c>
-      <c r="I20" t="n">
+      <c r="L20" t="n">
+        <v>0</v>
+      </c>
+      <c r="M20" t="n">
+        <v>0</v>
+      </c>
+      <c r="N20" t="n">
         <v>31.0654</v>
       </c>
-      <c r="J20" t="n">
-        <v>0</v>
-      </c>
-      <c r="K20" t="n">
+      <c r="O20" t="n">
+        <v>0</v>
+      </c>
+      <c r="P20" t="n">
         <v>9.933199999999999</v>
       </c>
-      <c r="L20" t="n">
-        <v>0</v>
-      </c>
-      <c r="M20" t="n">
+      <c r="Q20" t="n">
+        <v>0</v>
+      </c>
+      <c r="R20" t="n">
         <v>4.3456</v>
       </c>
-      <c r="N20" t="n">
-        <v>0</v>
-      </c>
-      <c r="O20" t="n">
-        <v>0</v>
-      </c>
-      <c r="P20" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q20" t="n">
-        <v>0</v>
-      </c>
-      <c r="R20" t="inlineStr">
+      <c r="S20" t="n">
+        <v>0</v>
+      </c>
+      <c r="T20" t="n">
+        <v>0</v>
+      </c>
+      <c r="U20" t="n">
+        <v>2</v>
+      </c>
+      <c r="V20" t="n">
+        <v>0</v>
+      </c>
+      <c r="W20" t="inlineStr">
         <is>
           <t>07/24/2024</t>
         </is>
       </c>
-      <c r="S20" t="inlineStr">
+      <c r="X20" t="inlineStr">
         <is>
           <t>17:56:55</t>
         </is>
@@ -3099,51 +3126,51 @@
       <c r="D21" t="n">
         <v>0</v>
       </c>
-      <c r="E21" t="n">
-        <v>0</v>
-      </c>
-      <c r="F21" t="n">
-        <v>0</v>
-      </c>
       <c r="G21" t="n">
         <v>0</v>
       </c>
       <c r="H21" t="n">
         <v>0</v>
       </c>
-      <c r="I21" t="n">
+      <c r="L21" t="n">
+        <v>0</v>
+      </c>
+      <c r="M21" t="n">
+        <v>0</v>
+      </c>
+      <c r="N21" t="n">
         <v>31.0654</v>
       </c>
-      <c r="J21" t="n">
-        <v>0</v>
-      </c>
-      <c r="K21" t="n">
+      <c r="O21" t="n">
+        <v>0</v>
+      </c>
+      <c r="P21" t="n">
         <v>9.933199999999999</v>
       </c>
-      <c r="L21" t="n">
-        <v>0</v>
-      </c>
-      <c r="M21" t="n">
+      <c r="Q21" t="n">
+        <v>0</v>
+      </c>
+      <c r="R21" t="n">
         <v>4.3456</v>
       </c>
-      <c r="N21" t="n">
-        <v>0</v>
-      </c>
-      <c r="O21" t="n">
-        <v>0</v>
-      </c>
-      <c r="P21" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q21" t="n">
-        <v>0</v>
-      </c>
-      <c r="R21" t="inlineStr">
+      <c r="S21" t="n">
+        <v>0</v>
+      </c>
+      <c r="T21" t="n">
+        <v>0</v>
+      </c>
+      <c r="U21" t="n">
+        <v>2</v>
+      </c>
+      <c r="V21" t="n">
+        <v>0</v>
+      </c>
+      <c r="W21" t="inlineStr">
         <is>
           <t>07/25/2024</t>
         </is>
       </c>
-      <c r="S21" t="inlineStr">
+      <c r="X21" t="inlineStr">
         <is>
           <t>08:34:37</t>
         </is>
@@ -3162,56 +3189,56 @@
       <c r="D22" t="n">
         <v>0</v>
       </c>
-      <c r="E22" t="n">
-        <v>0</v>
-      </c>
-      <c r="F22" t="n">
-        <v>0</v>
-      </c>
       <c r="G22" t="n">
         <v>0</v>
       </c>
       <c r="H22" t="n">
         <v>0</v>
       </c>
-      <c r="I22" t="n">
+      <c r="L22" t="n">
+        <v>0</v>
+      </c>
+      <c r="M22" t="n">
+        <v>0</v>
+      </c>
+      <c r="N22" t="n">
         <v>31.0654</v>
       </c>
-      <c r="J22" t="n">
-        <v>0</v>
-      </c>
-      <c r="K22" t="n">
+      <c r="O22" t="n">
+        <v>0</v>
+      </c>
+      <c r="P22" t="n">
         <v>9.933199999999999</v>
       </c>
-      <c r="L22" t="n">
-        <v>0</v>
-      </c>
-      <c r="M22" t="n">
+      <c r="Q22" t="n">
+        <v>0</v>
+      </c>
+      <c r="R22" t="n">
         <v>4.3456</v>
       </c>
-      <c r="N22" t="n">
-        <v>0</v>
-      </c>
-      <c r="O22" t="n">
-        <v>0</v>
-      </c>
-      <c r="P22" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q22" t="n">
-        <v>0</v>
-      </c>
-      <c r="R22" t="inlineStr">
+      <c r="S22" t="n">
+        <v>0</v>
+      </c>
+      <c r="T22" t="n">
+        <v>0</v>
+      </c>
+      <c r="U22" t="n">
+        <v>2</v>
+      </c>
+      <c r="V22" t="n">
+        <v>0</v>
+      </c>
+      <c r="W22" t="inlineStr">
         <is>
           <t>07/25/2024</t>
         </is>
       </c>
-      <c r="S22" t="inlineStr">
+      <c r="X22" t="inlineStr">
         <is>
           <t>08:35:01</t>
         </is>
       </c>
-      <c r="T22" t="inlineStr">
+      <c r="Y22" t="inlineStr">
         <is>
           <t>05648231</t>
         </is>
@@ -3230,51 +3257,51 @@
       <c r="D23" t="n">
         <v>0.00476527784788</v>
       </c>
-      <c r="E23" t="n">
-        <v>0</v>
-      </c>
-      <c r="F23" t="n">
-        <v>0</v>
-      </c>
       <c r="G23" t="n">
         <v>0</v>
       </c>
       <c r="H23" t="n">
         <v>0</v>
       </c>
-      <c r="I23" t="n">
+      <c r="L23" t="n">
+        <v>0</v>
+      </c>
+      <c r="M23" t="n">
+        <v>0</v>
+      </c>
+      <c r="N23" t="n">
         <v>31.0654</v>
       </c>
-      <c r="J23" t="n">
-        <v>0</v>
-      </c>
-      <c r="K23" t="n">
+      <c r="O23" t="n">
+        <v>0</v>
+      </c>
+      <c r="P23" t="n">
         <v>9.933199999999999</v>
       </c>
-      <c r="L23" t="n">
-        <v>0</v>
-      </c>
-      <c r="M23" t="n">
+      <c r="Q23" t="n">
+        <v>0</v>
+      </c>
+      <c r="R23" t="n">
         <v>4.3456</v>
       </c>
-      <c r="N23" t="n">
-        <v>0</v>
-      </c>
-      <c r="O23" t="n">
-        <v>0</v>
-      </c>
-      <c r="P23" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q23" t="n">
-        <v>0</v>
-      </c>
-      <c r="R23" t="inlineStr">
+      <c r="S23" t="n">
+        <v>0</v>
+      </c>
+      <c r="T23" t="n">
+        <v>0</v>
+      </c>
+      <c r="U23" t="n">
+        <v>2</v>
+      </c>
+      <c r="V23" t="n">
+        <v>0</v>
+      </c>
+      <c r="W23" t="inlineStr">
         <is>
           <t>07/25/2024</t>
         </is>
       </c>
-      <c r="S23" t="inlineStr">
+      <c r="X23" t="inlineStr">
         <is>
           <t>11:23:39</t>
         </is>
@@ -3293,51 +3320,51 @@
       <c r="D24" t="n">
         <v>0.006438130211520001</v>
       </c>
-      <c r="E24" t="n">
-        <v>0</v>
-      </c>
-      <c r="F24" t="n">
-        <v>0</v>
-      </c>
       <c r="G24" t="n">
         <v>0</v>
       </c>
       <c r="H24" t="n">
         <v>0</v>
       </c>
-      <c r="I24" t="n">
+      <c r="L24" t="n">
+        <v>0</v>
+      </c>
+      <c r="M24" t="n">
+        <v>0</v>
+      </c>
+      <c r="N24" t="n">
         <v>31.0654</v>
       </c>
-      <c r="J24" t="n">
-        <v>0</v>
-      </c>
-      <c r="K24" t="n">
+      <c r="O24" t="n">
+        <v>0</v>
+      </c>
+      <c r="P24" t="n">
         <v>9.933199999999999</v>
       </c>
-      <c r="L24" t="n">
-        <v>0</v>
-      </c>
-      <c r="M24" t="n">
+      <c r="Q24" t="n">
+        <v>0</v>
+      </c>
+      <c r="R24" t="n">
         <v>4.3456</v>
       </c>
-      <c r="N24" t="n">
-        <v>0</v>
-      </c>
-      <c r="O24" t="n">
-        <v>0</v>
-      </c>
-      <c r="P24" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q24" t="n">
-        <v>0</v>
-      </c>
-      <c r="R24" t="inlineStr">
+      <c r="S24" t="n">
+        <v>0</v>
+      </c>
+      <c r="T24" t="n">
+        <v>0</v>
+      </c>
+      <c r="U24" t="n">
+        <v>2</v>
+      </c>
+      <c r="V24" t="n">
+        <v>0</v>
+      </c>
+      <c r="W24" t="inlineStr">
         <is>
           <t>07/25/2024</t>
         </is>
       </c>
-      <c r="S24" t="inlineStr">
+      <c r="X24" t="inlineStr">
         <is>
           <t>11:24:07</t>
         </is>
@@ -3356,51 +3383,51 @@
       <c r="D25" t="n">
         <v>0</v>
       </c>
-      <c r="E25" t="n">
-        <v>0</v>
-      </c>
-      <c r="F25" t="n">
-        <v>0</v>
-      </c>
       <c r="G25" t="n">
         <v>0</v>
       </c>
       <c r="H25" t="n">
         <v>0</v>
       </c>
-      <c r="I25" t="n">
+      <c r="L25" t="n">
+        <v>0</v>
+      </c>
+      <c r="M25" t="n">
+        <v>0</v>
+      </c>
+      <c r="N25" t="n">
         <v>31.0654</v>
       </c>
-      <c r="J25" t="n">
-        <v>0</v>
-      </c>
-      <c r="K25" t="n">
+      <c r="O25" t="n">
+        <v>0</v>
+      </c>
+      <c r="P25" t="n">
         <v>9.933199999999999</v>
       </c>
-      <c r="L25" t="n">
-        <v>0</v>
-      </c>
-      <c r="M25" t="n">
+      <c r="Q25" t="n">
+        <v>0</v>
+      </c>
+      <c r="R25" t="n">
         <v>4.3456</v>
       </c>
-      <c r="N25" t="n">
-        <v>0</v>
-      </c>
-      <c r="O25" t="n">
-        <v>0</v>
-      </c>
-      <c r="P25" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q25" t="n">
-        <v>0</v>
-      </c>
-      <c r="R25" t="inlineStr">
+      <c r="S25" t="n">
+        <v>0</v>
+      </c>
+      <c r="T25" t="n">
+        <v>0</v>
+      </c>
+      <c r="U25" t="n">
+        <v>2</v>
+      </c>
+      <c r="V25" t="n">
+        <v>0</v>
+      </c>
+      <c r="W25" t="inlineStr">
         <is>
           <t>07/27/2024</t>
         </is>
       </c>
-      <c r="S25" t="inlineStr">
+      <c r="X25" t="inlineStr">
         <is>
           <t>20:16:37</t>
         </is>
@@ -3419,51 +3446,51 @@
       <c r="D26" t="n">
         <v>0</v>
       </c>
-      <c r="E26" t="n">
-        <v>0</v>
-      </c>
-      <c r="F26" t="n">
-        <v>0</v>
-      </c>
       <c r="G26" t="n">
         <v>0</v>
       </c>
       <c r="H26" t="n">
         <v>0</v>
       </c>
-      <c r="I26" t="n">
+      <c r="L26" t="n">
+        <v>0</v>
+      </c>
+      <c r="M26" t="n">
+        <v>0</v>
+      </c>
+      <c r="N26" t="n">
         <v>31.0654</v>
       </c>
-      <c r="J26" t="n">
-        <v>0</v>
-      </c>
-      <c r="K26" t="n">
+      <c r="O26" t="n">
+        <v>0</v>
+      </c>
+      <c r="P26" t="n">
         <v>9.933199999999999</v>
       </c>
-      <c r="L26" t="n">
-        <v>0</v>
-      </c>
-      <c r="M26" t="n">
+      <c r="Q26" t="n">
+        <v>0</v>
+      </c>
+      <c r="R26" t="n">
         <v>4.3456</v>
       </c>
-      <c r="N26" t="n">
-        <v>0</v>
-      </c>
-      <c r="O26" t="n">
-        <v>0</v>
-      </c>
-      <c r="P26" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q26" t="n">
-        <v>0</v>
-      </c>
-      <c r="R26" t="inlineStr">
+      <c r="S26" t="n">
+        <v>0</v>
+      </c>
+      <c r="T26" t="n">
+        <v>0</v>
+      </c>
+      <c r="U26" t="n">
+        <v>2</v>
+      </c>
+      <c r="V26" t="n">
+        <v>0</v>
+      </c>
+      <c r="W26" t="inlineStr">
         <is>
           <t>07/29/2024</t>
         </is>
       </c>
-      <c r="S26" t="inlineStr">
+      <c r="X26" t="inlineStr">
         <is>
           <t>21:17:30</t>
         </is>
@@ -3482,51 +3509,51 @@
       <c r="D27" t="n">
         <v>0</v>
       </c>
-      <c r="E27" t="n">
-        <v>0</v>
-      </c>
-      <c r="F27" t="n">
-        <v>0</v>
-      </c>
       <c r="G27" t="n">
         <v>0</v>
       </c>
       <c r="H27" t="n">
         <v>0</v>
       </c>
-      <c r="I27" t="n">
+      <c r="L27" t="n">
+        <v>0</v>
+      </c>
+      <c r="M27" t="n">
+        <v>0</v>
+      </c>
+      <c r="N27" t="n">
         <v>31.0654</v>
       </c>
-      <c r="J27" t="n">
-        <v>0</v>
-      </c>
-      <c r="K27" t="n">
+      <c r="O27" t="n">
+        <v>0</v>
+      </c>
+      <c r="P27" t="n">
         <v>9.933199999999999</v>
       </c>
-      <c r="L27" t="n">
-        <v>0</v>
-      </c>
-      <c r="M27" t="n">
+      <c r="Q27" t="n">
+        <v>0</v>
+      </c>
+      <c r="R27" t="n">
         <v>4.3456</v>
       </c>
-      <c r="N27" t="n">
-        <v>0</v>
-      </c>
-      <c r="O27" t="n">
-        <v>0</v>
-      </c>
-      <c r="P27" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q27" t="n">
-        <v>0</v>
-      </c>
-      <c r="R27" t="inlineStr">
+      <c r="S27" t="n">
+        <v>0</v>
+      </c>
+      <c r="T27" t="n">
+        <v>0</v>
+      </c>
+      <c r="U27" t="n">
+        <v>2</v>
+      </c>
+      <c r="V27" t="n">
+        <v>0</v>
+      </c>
+      <c r="W27" t="inlineStr">
         <is>
           <t>07/29/2024</t>
         </is>
       </c>
-      <c r="S27" t="inlineStr">
+      <c r="X27" t="inlineStr">
         <is>
           <t>21:17:48</t>
         </is>
@@ -3545,51 +3572,51 @@
       <c r="D28" t="n">
         <v>0</v>
       </c>
-      <c r="E28" t="n">
-        <v>0</v>
-      </c>
-      <c r="F28" t="n">
-        <v>0</v>
-      </c>
       <c r="G28" t="n">
         <v>0</v>
       </c>
       <c r="H28" t="n">
         <v>0</v>
       </c>
-      <c r="I28" t="n">
+      <c r="L28" t="n">
+        <v>0</v>
+      </c>
+      <c r="M28" t="n">
+        <v>0</v>
+      </c>
+      <c r="N28" t="n">
         <v>31.0654</v>
       </c>
-      <c r="J28" t="n">
-        <v>0</v>
-      </c>
-      <c r="K28" t="n">
+      <c r="O28" t="n">
+        <v>0</v>
+      </c>
+      <c r="P28" t="n">
         <v>9.933199999999999</v>
       </c>
-      <c r="L28" t="n">
-        <v>0</v>
-      </c>
-      <c r="M28" t="n">
+      <c r="Q28" t="n">
+        <v>0</v>
+      </c>
+      <c r="R28" t="n">
         <v>4.3456</v>
       </c>
-      <c r="N28" t="n">
-        <v>0</v>
-      </c>
-      <c r="O28" t="n">
-        <v>0</v>
-      </c>
-      <c r="P28" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q28" t="n">
-        <v>0</v>
-      </c>
-      <c r="R28" t="inlineStr">
+      <c r="S28" t="n">
+        <v>0</v>
+      </c>
+      <c r="T28" t="n">
+        <v>0</v>
+      </c>
+      <c r="U28" t="n">
+        <v>2</v>
+      </c>
+      <c r="V28" t="n">
+        <v>0</v>
+      </c>
+      <c r="W28" t="inlineStr">
         <is>
           <t>07/29/2024</t>
         </is>
       </c>
-      <c r="S28" t="inlineStr">
+      <c r="X28" t="inlineStr">
         <is>
           <t>21:31:08</t>
         </is>
@@ -3608,51 +3635,51 @@
       <c r="D29" t="n">
         <v>0</v>
       </c>
-      <c r="E29" t="n">
-        <v>0</v>
-      </c>
-      <c r="F29" t="n">
-        <v>0</v>
-      </c>
       <c r="G29" t="n">
         <v>0</v>
       </c>
       <c r="H29" t="n">
         <v>0</v>
       </c>
-      <c r="I29" t="n">
+      <c r="L29" t="n">
+        <v>0</v>
+      </c>
+      <c r="M29" t="n">
+        <v>0</v>
+      </c>
+      <c r="N29" t="n">
         <v>31.0654</v>
       </c>
-      <c r="J29" t="n">
-        <v>0</v>
-      </c>
-      <c r="K29" t="n">
+      <c r="O29" t="n">
+        <v>0</v>
+      </c>
+      <c r="P29" t="n">
         <v>9.933199999999999</v>
       </c>
-      <c r="L29" t="n">
-        <v>0</v>
-      </c>
-      <c r="M29" t="n">
+      <c r="Q29" t="n">
+        <v>0</v>
+      </c>
+      <c r="R29" t="n">
         <v>4.3456</v>
       </c>
-      <c r="N29" t="n">
-        <v>0</v>
-      </c>
-      <c r="O29" t="n">
-        <v>0</v>
-      </c>
-      <c r="P29" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q29" t="n">
-        <v>0</v>
-      </c>
-      <c r="R29" t="inlineStr">
+      <c r="S29" t="n">
+        <v>0</v>
+      </c>
+      <c r="T29" t="n">
+        <v>0</v>
+      </c>
+      <c r="U29" t="n">
+        <v>2</v>
+      </c>
+      <c r="V29" t="n">
+        <v>0</v>
+      </c>
+      <c r="W29" t="inlineStr">
         <is>
           <t>07/29/2024</t>
         </is>
       </c>
-      <c r="S29" t="inlineStr">
+      <c r="X29" t="inlineStr">
         <is>
           <t>21:39:14</t>
         </is>
@@ -3671,51 +3698,51 @@
       <c r="D30" t="n">
         <v>0</v>
       </c>
-      <c r="E30" t="n">
-        <v>0</v>
-      </c>
-      <c r="F30" t="n">
-        <v>0</v>
-      </c>
       <c r="G30" t="n">
         <v>0</v>
       </c>
       <c r="H30" t="n">
         <v>0</v>
       </c>
-      <c r="I30" t="n">
+      <c r="L30" t="n">
+        <v>0</v>
+      </c>
+      <c r="M30" t="n">
+        <v>0</v>
+      </c>
+      <c r="N30" t="n">
         <v>31.0654</v>
       </c>
-      <c r="J30" t="n">
-        <v>0</v>
-      </c>
-      <c r="K30" t="n">
+      <c r="O30" t="n">
+        <v>0</v>
+      </c>
+      <c r="P30" t="n">
         <v>9.933199999999999</v>
       </c>
-      <c r="L30" t="n">
-        <v>0</v>
-      </c>
-      <c r="M30" t="n">
+      <c r="Q30" t="n">
+        <v>0</v>
+      </c>
+      <c r="R30" t="n">
         <v>4.3456</v>
       </c>
-      <c r="N30" t="n">
-        <v>0</v>
-      </c>
-      <c r="O30" t="n">
-        <v>0</v>
-      </c>
-      <c r="P30" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q30" t="n">
-        <v>0</v>
-      </c>
-      <c r="R30" t="inlineStr">
+      <c r="S30" t="n">
+        <v>0</v>
+      </c>
+      <c r="T30" t="n">
+        <v>0</v>
+      </c>
+      <c r="U30" t="n">
+        <v>2</v>
+      </c>
+      <c r="V30" t="n">
+        <v>0</v>
+      </c>
+      <c r="W30" t="inlineStr">
         <is>
           <t>07/29/2024</t>
         </is>
       </c>
-      <c r="S30" t="inlineStr">
+      <c r="X30" t="inlineStr">
         <is>
           <t>23:05:27</t>
         </is>
@@ -3734,51 +3761,51 @@
       <c r="D31" t="n">
         <v>0</v>
       </c>
-      <c r="E31" t="n">
-        <v>0</v>
-      </c>
-      <c r="F31" t="n">
-        <v>0</v>
-      </c>
       <c r="G31" t="n">
         <v>0</v>
       </c>
       <c r="H31" t="n">
         <v>0</v>
       </c>
-      <c r="I31" t="n">
+      <c r="L31" t="n">
+        <v>0</v>
+      </c>
+      <c r="M31" t="n">
+        <v>0</v>
+      </c>
+      <c r="N31" t="n">
         <v>31.0654</v>
       </c>
-      <c r="J31" t="n">
-        <v>0</v>
-      </c>
-      <c r="K31" t="n">
+      <c r="O31" t="n">
+        <v>0</v>
+      </c>
+      <c r="P31" t="n">
         <v>9.933199999999999</v>
       </c>
-      <c r="L31" t="n">
-        <v>0</v>
-      </c>
-      <c r="M31" t="n">
+      <c r="Q31" t="n">
+        <v>0</v>
+      </c>
+      <c r="R31" t="n">
         <v>4.3456</v>
       </c>
-      <c r="N31" t="n">
-        <v>0</v>
-      </c>
-      <c r="O31" t="n">
-        <v>0</v>
-      </c>
-      <c r="P31" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q31" t="n">
-        <v>0</v>
-      </c>
-      <c r="R31" t="inlineStr">
+      <c r="S31" t="n">
+        <v>0</v>
+      </c>
+      <c r="T31" t="n">
+        <v>0</v>
+      </c>
+      <c r="U31" t="n">
+        <v>2</v>
+      </c>
+      <c r="V31" t="n">
+        <v>0</v>
+      </c>
+      <c r="W31" t="inlineStr">
         <is>
           <t>07/30/2024</t>
         </is>
       </c>
-      <c r="S31" t="inlineStr">
+      <c r="X31" t="inlineStr">
         <is>
           <t>11:39:35</t>
         </is>
@@ -3797,51 +3824,51 @@
       <c r="D32" t="n">
         <v>0</v>
       </c>
-      <c r="E32" t="n">
-        <v>0</v>
-      </c>
-      <c r="F32" t="n">
-        <v>0</v>
-      </c>
       <c r="G32" t="n">
         <v>0</v>
       </c>
       <c r="H32" t="n">
         <v>0</v>
       </c>
-      <c r="I32" t="n">
+      <c r="L32" t="n">
+        <v>0</v>
+      </c>
+      <c r="M32" t="n">
+        <v>0</v>
+      </c>
+      <c r="N32" t="n">
         <v>31.0654</v>
       </c>
-      <c r="J32" t="n">
-        <v>0</v>
-      </c>
-      <c r="K32" t="n">
+      <c r="O32" t="n">
+        <v>0</v>
+      </c>
+      <c r="P32" t="n">
         <v>9.933199999999999</v>
       </c>
-      <c r="L32" t="n">
-        <v>0</v>
-      </c>
-      <c r="M32" t="n">
+      <c r="Q32" t="n">
+        <v>0</v>
+      </c>
+      <c r="R32" t="n">
         <v>4.3456</v>
       </c>
-      <c r="N32" t="n">
-        <v>0</v>
-      </c>
-      <c r="O32" t="n">
-        <v>0</v>
-      </c>
-      <c r="P32" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q32" t="n">
-        <v>0</v>
-      </c>
-      <c r="R32" t="inlineStr">
+      <c r="S32" t="n">
+        <v>0</v>
+      </c>
+      <c r="T32" t="n">
+        <v>0</v>
+      </c>
+      <c r="U32" t="n">
+        <v>2</v>
+      </c>
+      <c r="V32" t="n">
+        <v>0</v>
+      </c>
+      <c r="W32" t="inlineStr">
         <is>
           <t>07/30/2024</t>
         </is>
       </c>
-      <c r="S32" t="inlineStr">
+      <c r="X32" t="inlineStr">
         <is>
           <t>11:41:39</t>
         </is>
@@ -3860,51 +3887,51 @@
       <c r="D33" t="n">
         <v>0</v>
       </c>
-      <c r="E33" t="n">
-        <v>0</v>
-      </c>
-      <c r="F33" t="n">
-        <v>0</v>
-      </c>
       <c r="G33" t="n">
         <v>0</v>
       </c>
       <c r="H33" t="n">
         <v>0</v>
       </c>
-      <c r="I33" t="n">
+      <c r="L33" t="n">
+        <v>0</v>
+      </c>
+      <c r="M33" t="n">
+        <v>0</v>
+      </c>
+      <c r="N33" t="n">
         <v>31.0654</v>
       </c>
-      <c r="J33" t="n">
-        <v>0</v>
-      </c>
-      <c r="K33" t="n">
+      <c r="O33" t="n">
+        <v>0</v>
+      </c>
+      <c r="P33" t="n">
         <v>9.933199999999999</v>
       </c>
-      <c r="L33" t="n">
-        <v>0</v>
-      </c>
-      <c r="M33" t="n">
+      <c r="Q33" t="n">
+        <v>0</v>
+      </c>
+      <c r="R33" t="n">
         <v>4.3456</v>
       </c>
-      <c r="N33" t="n">
-        <v>0</v>
-      </c>
-      <c r="O33" t="n">
-        <v>0</v>
-      </c>
-      <c r="P33" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q33" t="n">
-        <v>0</v>
-      </c>
-      <c r="R33" t="inlineStr">
+      <c r="S33" t="n">
+        <v>0</v>
+      </c>
+      <c r="T33" t="n">
+        <v>0</v>
+      </c>
+      <c r="U33" t="n">
+        <v>2</v>
+      </c>
+      <c r="V33" t="n">
+        <v>0</v>
+      </c>
+      <c r="W33" t="inlineStr">
         <is>
           <t>07/30/2024</t>
         </is>
       </c>
-      <c r="S33" t="inlineStr">
+      <c r="X33" t="inlineStr">
         <is>
           <t>11:42:37</t>
         </is>
@@ -3923,51 +3950,51 @@
       <c r="D34" t="n">
         <v>0</v>
       </c>
-      <c r="E34" t="n">
-        <v>0</v>
-      </c>
-      <c r="F34" t="n">
-        <v>0</v>
-      </c>
       <c r="G34" t="n">
         <v>0</v>
       </c>
       <c r="H34" t="n">
         <v>0</v>
       </c>
-      <c r="I34" t="n">
+      <c r="L34" t="n">
+        <v>0</v>
+      </c>
+      <c r="M34" t="n">
+        <v>0</v>
+      </c>
+      <c r="N34" t="n">
         <v>31.0654</v>
       </c>
-      <c r="J34" t="n">
-        <v>0</v>
-      </c>
-      <c r="K34" t="n">
+      <c r="O34" t="n">
+        <v>0</v>
+      </c>
+      <c r="P34" t="n">
         <v>9.933199999999999</v>
       </c>
-      <c r="L34" t="n">
-        <v>0</v>
-      </c>
-      <c r="M34" t="n">
+      <c r="Q34" t="n">
+        <v>0</v>
+      </c>
+      <c r="R34" t="n">
         <v>4.3456</v>
       </c>
-      <c r="N34" t="n">
-        <v>0</v>
-      </c>
-      <c r="O34" t="n">
-        <v>0</v>
-      </c>
-      <c r="P34" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q34" t="n">
-        <v>0</v>
-      </c>
-      <c r="R34" t="inlineStr">
+      <c r="S34" t="n">
+        <v>0</v>
+      </c>
+      <c r="T34" t="n">
+        <v>0</v>
+      </c>
+      <c r="U34" t="n">
+        <v>2</v>
+      </c>
+      <c r="V34" t="n">
+        <v>0</v>
+      </c>
+      <c r="W34" t="inlineStr">
         <is>
           <t>07/30/2024</t>
         </is>
       </c>
-      <c r="S34" t="inlineStr">
+      <c r="X34" t="inlineStr">
         <is>
           <t>11:45:09</t>
         </is>
@@ -3986,51 +4013,51 @@
       <c r="D35" t="n">
         <v>0</v>
       </c>
-      <c r="E35" t="n">
-        <v>0</v>
-      </c>
-      <c r="F35" t="n">
-        <v>0</v>
-      </c>
       <c r="G35" t="n">
         <v>0</v>
       </c>
       <c r="H35" t="n">
         <v>0</v>
       </c>
-      <c r="I35" t="n">
+      <c r="L35" t="n">
+        <v>0</v>
+      </c>
+      <c r="M35" t="n">
+        <v>0</v>
+      </c>
+      <c r="N35" t="n">
         <v>31.0654</v>
       </c>
-      <c r="J35" t="n">
-        <v>0</v>
-      </c>
-      <c r="K35" t="n">
+      <c r="O35" t="n">
+        <v>0</v>
+      </c>
+      <c r="P35" t="n">
         <v>9.933199999999999</v>
       </c>
-      <c r="L35" t="n">
-        <v>0</v>
-      </c>
-      <c r="M35" t="n">
+      <c r="Q35" t="n">
+        <v>0</v>
+      </c>
+      <c r="R35" t="n">
         <v>4.3456</v>
       </c>
-      <c r="N35" t="n">
-        <v>0</v>
-      </c>
-      <c r="O35" t="n">
-        <v>0</v>
-      </c>
-      <c r="P35" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q35" t="n">
-        <v>0</v>
-      </c>
-      <c r="R35" t="inlineStr">
+      <c r="S35" t="n">
+        <v>0</v>
+      </c>
+      <c r="T35" t="n">
+        <v>0</v>
+      </c>
+      <c r="U35" t="n">
+        <v>2</v>
+      </c>
+      <c r="V35" t="n">
+        <v>0</v>
+      </c>
+      <c r="W35" t="inlineStr">
         <is>
           <t>07/30/2024</t>
         </is>
       </c>
-      <c r="S35" t="inlineStr">
+      <c r="X35" t="inlineStr">
         <is>
           <t>11:46:17</t>
         </is>
@@ -4049,51 +4076,51 @@
       <c r="D36" t="n">
         <v>0</v>
       </c>
-      <c r="E36" t="n">
-        <v>0</v>
-      </c>
-      <c r="F36" t="n">
-        <v>0</v>
-      </c>
       <c r="G36" t="n">
         <v>0</v>
       </c>
       <c r="H36" t="n">
         <v>0</v>
       </c>
-      <c r="I36" t="n">
+      <c r="L36" t="n">
+        <v>0</v>
+      </c>
+      <c r="M36" t="n">
+        <v>0</v>
+      </c>
+      <c r="N36" t="n">
         <v>31.0654</v>
       </c>
-      <c r="J36" t="n">
-        <v>0</v>
-      </c>
-      <c r="K36" t="n">
+      <c r="O36" t="n">
+        <v>0</v>
+      </c>
+      <c r="P36" t="n">
         <v>9.933199999999999</v>
       </c>
-      <c r="L36" t="n">
-        <v>0</v>
-      </c>
-      <c r="M36" t="n">
+      <c r="Q36" t="n">
+        <v>0</v>
+      </c>
+      <c r="R36" t="n">
         <v>4.3456</v>
       </c>
-      <c r="N36" t="n">
-        <v>0</v>
-      </c>
-      <c r="O36" t="n">
-        <v>0</v>
-      </c>
-      <c r="P36" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q36" t="n">
-        <v>0</v>
-      </c>
-      <c r="R36" t="inlineStr">
+      <c r="S36" t="n">
+        <v>0</v>
+      </c>
+      <c r="T36" t="n">
+        <v>0</v>
+      </c>
+      <c r="U36" t="n">
+        <v>2</v>
+      </c>
+      <c r="V36" t="n">
+        <v>0</v>
+      </c>
+      <c r="W36" t="inlineStr">
         <is>
           <t>07/30/2024</t>
         </is>
       </c>
-      <c r="S36" t="inlineStr">
+      <c r="X36" t="inlineStr">
         <is>
           <t>12:04:10</t>
         </is>
@@ -4112,56 +4139,56 @@
       <c r="D37" t="n">
         <v>0</v>
       </c>
-      <c r="E37" t="n">
-        <v>0</v>
-      </c>
-      <c r="F37" t="n">
-        <v>0</v>
-      </c>
       <c r="G37" t="n">
         <v>0</v>
       </c>
       <c r="H37" t="n">
         <v>0</v>
       </c>
-      <c r="I37" t="n">
+      <c r="L37" t="n">
+        <v>0</v>
+      </c>
+      <c r="M37" t="n">
+        <v>0</v>
+      </c>
+      <c r="N37" t="n">
         <v>31.0654</v>
       </c>
-      <c r="J37" t="n">
-        <v>0</v>
-      </c>
-      <c r="K37" t="n">
+      <c r="O37" t="n">
+        <v>0</v>
+      </c>
+      <c r="P37" t="n">
         <v>9.933199999999999</v>
       </c>
-      <c r="L37" t="n">
-        <v>0</v>
-      </c>
-      <c r="M37" t="n">
+      <c r="Q37" t="n">
+        <v>0</v>
+      </c>
+      <c r="R37" t="n">
         <v>4.3456</v>
       </c>
-      <c r="N37" t="n">
-        <v>0</v>
-      </c>
-      <c r="O37" t="n">
-        <v>0</v>
-      </c>
-      <c r="P37" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q37" t="n">
-        <v>0</v>
-      </c>
-      <c r="R37" t="inlineStr">
+      <c r="S37" t="n">
+        <v>0</v>
+      </c>
+      <c r="T37" t="n">
+        <v>0</v>
+      </c>
+      <c r="U37" t="n">
+        <v>2</v>
+      </c>
+      <c r="V37" t="n">
+        <v>0</v>
+      </c>
+      <c r="W37" t="inlineStr">
         <is>
           <t>07/30/2024</t>
         </is>
       </c>
-      <c r="S37" t="inlineStr">
+      <c r="X37" t="inlineStr">
         <is>
           <t>12:04:31</t>
         </is>
       </c>
-      <c r="T37" t="inlineStr">
+      <c r="Y37" t="inlineStr">
         <is>
           <t>45325446</t>
         </is>
@@ -4180,56 +4207,56 @@
       <c r="D38" t="n">
         <v>0</v>
       </c>
-      <c r="E38" t="n">
-        <v>0</v>
-      </c>
-      <c r="F38" t="n">
-        <v>0</v>
-      </c>
       <c r="G38" t="n">
         <v>0</v>
       </c>
       <c r="H38" t="n">
         <v>0</v>
       </c>
-      <c r="I38" t="n">
+      <c r="L38" t="n">
+        <v>0</v>
+      </c>
+      <c r="M38" t="n">
+        <v>0</v>
+      </c>
+      <c r="N38" t="n">
         <v>31.0654</v>
       </c>
-      <c r="J38" t="n">
-        <v>0</v>
-      </c>
-      <c r="K38" t="n">
+      <c r="O38" t="n">
+        <v>0</v>
+      </c>
+      <c r="P38" t="n">
         <v>9.933199999999999</v>
       </c>
-      <c r="L38" t="n">
-        <v>0</v>
-      </c>
-      <c r="M38" t="n">
+      <c r="Q38" t="n">
+        <v>0</v>
+      </c>
+      <c r="R38" t="n">
         <v>4.3456</v>
       </c>
-      <c r="N38" t="n">
-        <v>0</v>
-      </c>
-      <c r="O38" t="n">
-        <v>0</v>
-      </c>
-      <c r="P38" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q38" t="n">
-        <v>0</v>
-      </c>
-      <c r="R38" t="inlineStr">
+      <c r="S38" t="n">
+        <v>0</v>
+      </c>
+      <c r="T38" t="n">
+        <v>0</v>
+      </c>
+      <c r="U38" t="n">
+        <v>2</v>
+      </c>
+      <c r="V38" t="n">
+        <v>0</v>
+      </c>
+      <c r="W38" t="inlineStr">
         <is>
           <t>07/30/2024</t>
         </is>
       </c>
-      <c r="S38" t="inlineStr">
+      <c r="X38" t="inlineStr">
         <is>
           <t>14:57:33</t>
         </is>
       </c>
-      <c r="T38" t="inlineStr">
+      <c r="Y38" t="inlineStr">
         <is>
           <t>32222222</t>
         </is>
@@ -4248,56 +4275,56 @@
       <c r="D39" t="n">
         <v>0</v>
       </c>
-      <c r="E39" t="n">
-        <v>0</v>
-      </c>
-      <c r="F39" t="n">
-        <v>0</v>
-      </c>
       <c r="G39" t="n">
         <v>0</v>
       </c>
       <c r="H39" t="n">
         <v>0</v>
       </c>
-      <c r="I39" t="n">
+      <c r="L39" t="n">
+        <v>0</v>
+      </c>
+      <c r="M39" t="n">
+        <v>0</v>
+      </c>
+      <c r="N39" t="n">
         <v>31.0654</v>
       </c>
-      <c r="J39" t="n">
-        <v>0</v>
-      </c>
-      <c r="K39" t="n">
+      <c r="O39" t="n">
+        <v>0</v>
+      </c>
+      <c r="P39" t="n">
         <v>9.933199999999999</v>
       </c>
-      <c r="L39" t="n">
-        <v>0</v>
-      </c>
-      <c r="M39" t="n">
+      <c r="Q39" t="n">
+        <v>0</v>
+      </c>
+      <c r="R39" t="n">
         <v>4.3456</v>
       </c>
-      <c r="N39" t="n">
-        <v>0</v>
-      </c>
-      <c r="O39" t="n">
-        <v>0</v>
-      </c>
-      <c r="P39" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q39" t="n">
-        <v>0</v>
-      </c>
-      <c r="R39" t="inlineStr">
+      <c r="S39" t="n">
+        <v>0</v>
+      </c>
+      <c r="T39" t="n">
+        <v>0</v>
+      </c>
+      <c r="U39" t="n">
+        <v>2</v>
+      </c>
+      <c r="V39" t="n">
+        <v>0</v>
+      </c>
+      <c r="W39" t="inlineStr">
         <is>
           <t>07/30/2024</t>
         </is>
       </c>
-      <c r="S39" t="inlineStr">
+      <c r="X39" t="inlineStr">
         <is>
           <t>14:57:44</t>
         </is>
       </c>
-      <c r="T39" t="inlineStr">
+      <c r="Y39" t="inlineStr">
         <is>
           <t>231111111</t>
         </is>
@@ -4316,56 +4343,56 @@
       <c r="D40" t="n">
         <v>0</v>
       </c>
-      <c r="E40" t="n">
-        <v>0</v>
-      </c>
-      <c r="F40" t="n">
-        <v>0</v>
-      </c>
       <c r="G40" t="n">
         <v>0</v>
       </c>
       <c r="H40" t="n">
         <v>0</v>
       </c>
-      <c r="I40" t="n">
+      <c r="L40" t="n">
+        <v>0</v>
+      </c>
+      <c r="M40" t="n">
+        <v>0</v>
+      </c>
+      <c r="N40" t="n">
         <v>31.0654</v>
       </c>
-      <c r="J40" t="n">
-        <v>0</v>
-      </c>
-      <c r="K40" t="n">
+      <c r="O40" t="n">
+        <v>0</v>
+      </c>
+      <c r="P40" t="n">
         <v>9.933199999999999</v>
       </c>
-      <c r="L40" t="n">
-        <v>0</v>
-      </c>
-      <c r="M40" t="n">
+      <c r="Q40" t="n">
+        <v>0</v>
+      </c>
+      <c r="R40" t="n">
         <v>4.3456</v>
       </c>
-      <c r="N40" t="n">
-        <v>0</v>
-      </c>
-      <c r="O40" t="n">
-        <v>0</v>
-      </c>
-      <c r="P40" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q40" t="n">
-        <v>0</v>
-      </c>
-      <c r="R40" t="inlineStr">
+      <c r="S40" t="n">
+        <v>0</v>
+      </c>
+      <c r="T40" t="n">
+        <v>0</v>
+      </c>
+      <c r="U40" t="n">
+        <v>2</v>
+      </c>
+      <c r="V40" t="n">
+        <v>0</v>
+      </c>
+      <c r="W40" t="inlineStr">
         <is>
           <t>07/30/2024</t>
         </is>
       </c>
-      <c r="S40" t="inlineStr">
+      <c r="X40" t="inlineStr">
         <is>
           <t>14:57:50</t>
         </is>
       </c>
-      <c r="T40" t="inlineStr">
+      <c r="Y40" t="inlineStr">
         <is>
           <t>2311114444</t>
         </is>
@@ -4384,56 +4411,56 @@
       <c r="D41" t="n">
         <v>0</v>
       </c>
-      <c r="E41" t="n">
-        <v>0</v>
-      </c>
-      <c r="F41" t="n">
-        <v>0</v>
-      </c>
       <c r="G41" t="n">
         <v>0</v>
       </c>
       <c r="H41" t="n">
         <v>0</v>
       </c>
-      <c r="I41" t="n">
+      <c r="L41" t="n">
+        <v>0</v>
+      </c>
+      <c r="M41" t="n">
+        <v>0</v>
+      </c>
+      <c r="N41" t="n">
         <v>31.0654</v>
       </c>
-      <c r="J41" t="n">
-        <v>0</v>
-      </c>
-      <c r="K41" t="n">
+      <c r="O41" t="n">
+        <v>0</v>
+      </c>
+      <c r="P41" t="n">
         <v>9.933199999999999</v>
       </c>
-      <c r="L41" t="n">
-        <v>0</v>
-      </c>
-      <c r="M41" t="n">
+      <c r="Q41" t="n">
+        <v>0</v>
+      </c>
+      <c r="R41" t="n">
         <v>4.3456</v>
       </c>
-      <c r="N41" t="n">
-        <v>0</v>
-      </c>
-      <c r="O41" t="n">
-        <v>0</v>
-      </c>
-      <c r="P41" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q41" t="n">
-        <v>0</v>
-      </c>
-      <c r="R41" t="inlineStr">
+      <c r="S41" t="n">
+        <v>0</v>
+      </c>
+      <c r="T41" t="n">
+        <v>0</v>
+      </c>
+      <c r="U41" t="n">
+        <v>2</v>
+      </c>
+      <c r="V41" t="n">
+        <v>0</v>
+      </c>
+      <c r="W41" t="inlineStr">
         <is>
           <t>07/30/2024</t>
         </is>
       </c>
-      <c r="S41" t="inlineStr">
+      <c r="X41" t="inlineStr">
         <is>
           <t>15:03:39</t>
         </is>
       </c>
-      <c r="T41" t="inlineStr">
+      <c r="Y41" t="inlineStr">
         <is>
           <t>2311114444</t>
         </is>
@@ -4452,51 +4479,51 @@
       <c r="D42" t="n">
         <v>105.0314285152173</v>
       </c>
-      <c r="E42" t="n">
-        <v>0</v>
-      </c>
-      <c r="F42" t="n">
-        <v>0</v>
-      </c>
       <c r="G42" t="n">
         <v>0</v>
       </c>
       <c r="H42" t="n">
         <v>0</v>
       </c>
-      <c r="I42" t="n">
+      <c r="L42" t="n">
+        <v>0</v>
+      </c>
+      <c r="M42" t="n">
+        <v>0</v>
+      </c>
+      <c r="N42" t="n">
         <v>31.0654</v>
       </c>
-      <c r="J42" t="n">
-        <v>0</v>
-      </c>
-      <c r="K42" t="n">
+      <c r="O42" t="n">
+        <v>0</v>
+      </c>
+      <c r="P42" t="n">
         <v>9.933199999999999</v>
       </c>
-      <c r="L42" t="n">
-        <v>0</v>
-      </c>
-      <c r="M42" t="n">
+      <c r="Q42" t="n">
+        <v>0</v>
+      </c>
+      <c r="R42" t="n">
         <v>4.3456</v>
       </c>
-      <c r="N42" t="n">
-        <v>0</v>
-      </c>
-      <c r="O42" t="n">
-        <v>0</v>
-      </c>
-      <c r="P42" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q42" t="n">
-        <v>0</v>
-      </c>
-      <c r="R42" t="inlineStr">
+      <c r="S42" t="n">
+        <v>0</v>
+      </c>
+      <c r="T42" t="n">
+        <v>0</v>
+      </c>
+      <c r="U42" t="n">
+        <v>2</v>
+      </c>
+      <c r="V42" t="n">
+        <v>0</v>
+      </c>
+      <c r="W42" t="inlineStr">
         <is>
           <t>07/30/2024</t>
         </is>
       </c>
-      <c r="S42" t="inlineStr">
+      <c r="X42" t="inlineStr">
         <is>
           <t>15:08:29</t>
         </is>
@@ -4515,56 +4542,56 @@
       <c r="D43" t="n">
         <v>107.910093893161</v>
       </c>
-      <c r="E43" t="n">
-        <v>0</v>
-      </c>
-      <c r="F43" t="n">
-        <v>0</v>
-      </c>
       <c r="G43" t="n">
         <v>0</v>
       </c>
       <c r="H43" t="n">
         <v>0</v>
       </c>
-      <c r="I43" t="n">
+      <c r="L43" t="n">
+        <v>0</v>
+      </c>
+      <c r="M43" t="n">
+        <v>0</v>
+      </c>
+      <c r="N43" t="n">
         <v>31.0654</v>
       </c>
-      <c r="J43" t="n">
-        <v>0</v>
-      </c>
-      <c r="K43" t="n">
+      <c r="O43" t="n">
+        <v>0</v>
+      </c>
+      <c r="P43" t="n">
         <v>9.933199999999999</v>
       </c>
-      <c r="L43" t="n">
-        <v>0</v>
-      </c>
-      <c r="M43" t="n">
+      <c r="Q43" t="n">
+        <v>0</v>
+      </c>
+      <c r="R43" t="n">
         <v>4.3456</v>
       </c>
-      <c r="N43" t="n">
-        <v>0</v>
-      </c>
-      <c r="O43" t="n">
-        <v>0</v>
-      </c>
-      <c r="P43" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q43" t="n">
-        <v>0</v>
-      </c>
-      <c r="R43" t="inlineStr">
+      <c r="S43" t="n">
+        <v>0</v>
+      </c>
+      <c r="T43" t="n">
+        <v>0</v>
+      </c>
+      <c r="U43" t="n">
+        <v>2</v>
+      </c>
+      <c r="V43" t="n">
+        <v>0</v>
+      </c>
+      <c r="W43" t="inlineStr">
         <is>
           <t>07/30/2024</t>
         </is>
       </c>
-      <c r="S43" t="inlineStr">
+      <c r="X43" t="inlineStr">
         <is>
           <t>15:08:35</t>
         </is>
       </c>
-      <c r="T43" t="inlineStr">
+      <c r="Y43" t="inlineStr">
         <is>
           <t>33322222</t>
         </is>
@@ -4583,56 +4610,56 @@
       <c r="D44" t="n">
         <v>111.3187619064996</v>
       </c>
-      <c r="E44" t="n">
-        <v>0</v>
-      </c>
-      <c r="F44" t="n">
-        <v>0</v>
-      </c>
       <c r="G44" t="n">
         <v>0</v>
       </c>
       <c r="H44" t="n">
         <v>0</v>
       </c>
-      <c r="I44" t="n">
+      <c r="L44" t="n">
+        <v>0</v>
+      </c>
+      <c r="M44" t="n">
+        <v>0</v>
+      </c>
+      <c r="N44" t="n">
         <v>31.0654</v>
       </c>
-      <c r="J44" t="n">
-        <v>0</v>
-      </c>
-      <c r="K44" t="n">
+      <c r="O44" t="n">
+        <v>0</v>
+      </c>
+      <c r="P44" t="n">
         <v>9.933199999999999</v>
       </c>
-      <c r="L44" t="n">
-        <v>0</v>
-      </c>
-      <c r="M44" t="n">
+      <c r="Q44" t="n">
+        <v>0</v>
+      </c>
+      <c r="R44" t="n">
         <v>4.3456</v>
       </c>
-      <c r="N44" t="n">
-        <v>0</v>
-      </c>
-      <c r="O44" t="n">
-        <v>0</v>
-      </c>
-      <c r="P44" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q44" t="n">
-        <v>0</v>
-      </c>
-      <c r="R44" t="inlineStr">
+      <c r="S44" t="n">
+        <v>0</v>
+      </c>
+      <c r="T44" t="n">
+        <v>0</v>
+      </c>
+      <c r="U44" t="n">
+        <v>2</v>
+      </c>
+      <c r="V44" t="n">
+        <v>0</v>
+      </c>
+      <c r="W44" t="inlineStr">
         <is>
           <t>07/30/2024</t>
         </is>
       </c>
-      <c r="S44" t="inlineStr">
+      <c r="X44" t="inlineStr">
         <is>
           <t>15:08:36</t>
         </is>
       </c>
-      <c r="T44" t="inlineStr">
+      <c r="Y44" t="inlineStr">
         <is>
           <t>33322222</t>
         </is>
@@ -4651,56 +4678,56 @@
       <c r="D45" t="n">
         <v>111.3187619064996</v>
       </c>
-      <c r="E45" t="n">
-        <v>0</v>
-      </c>
-      <c r="F45" t="n">
-        <v>0</v>
-      </c>
       <c r="G45" t="n">
         <v>0</v>
       </c>
       <c r="H45" t="n">
         <v>0</v>
       </c>
-      <c r="I45" t="n">
+      <c r="L45" t="n">
+        <v>0</v>
+      </c>
+      <c r="M45" t="n">
+        <v>0</v>
+      </c>
+      <c r="N45" t="n">
         <v>31.0654</v>
       </c>
-      <c r="J45" t="n">
-        <v>0</v>
-      </c>
-      <c r="K45" t="n">
+      <c r="O45" t="n">
+        <v>0</v>
+      </c>
+      <c r="P45" t="n">
         <v>9.933199999999999</v>
       </c>
-      <c r="L45" t="n">
-        <v>0</v>
-      </c>
-      <c r="M45" t="n">
+      <c r="Q45" t="n">
+        <v>0</v>
+      </c>
+      <c r="R45" t="n">
         <v>4.3456</v>
       </c>
-      <c r="N45" t="n">
-        <v>0</v>
-      </c>
-      <c r="O45" t="n">
-        <v>0</v>
-      </c>
-      <c r="P45" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q45" t="n">
-        <v>0</v>
-      </c>
-      <c r="R45" t="inlineStr">
+      <c r="S45" t="n">
+        <v>0</v>
+      </c>
+      <c r="T45" t="n">
+        <v>0</v>
+      </c>
+      <c r="U45" t="n">
+        <v>2</v>
+      </c>
+      <c r="V45" t="n">
+        <v>0</v>
+      </c>
+      <c r="W45" t="inlineStr">
         <is>
           <t>07/30/2024</t>
         </is>
       </c>
-      <c r="S45" t="inlineStr">
+      <c r="X45" t="inlineStr">
         <is>
           <t>15:08:39</t>
         </is>
       </c>
-      <c r="T45" t="inlineStr">
+      <c r="Y45" t="inlineStr">
         <is>
           <t>33322222</t>
         </is>
@@ -4719,60 +4746,138 @@
       <c r="D46" t="n">
         <v>113.9469328977034</v>
       </c>
-      <c r="E46" t="n">
-        <v>0</v>
-      </c>
-      <c r="F46" t="n">
-        <v>0</v>
-      </c>
       <c r="G46" t="n">
         <v>0</v>
       </c>
       <c r="H46" t="n">
         <v>0</v>
       </c>
-      <c r="I46" t="n">
+      <c r="L46" t="n">
+        <v>0</v>
+      </c>
+      <c r="M46" t="n">
+        <v>0</v>
+      </c>
+      <c r="N46" t="n">
         <v>31.0654</v>
       </c>
-      <c r="J46" t="n">
-        <v>0</v>
-      </c>
-      <c r="K46" t="n">
+      <c r="O46" t="n">
+        <v>0</v>
+      </c>
+      <c r="P46" t="n">
         <v>9.933199999999999</v>
       </c>
-      <c r="L46" t="n">
-        <v>0</v>
-      </c>
-      <c r="M46" t="n">
+      <c r="Q46" t="n">
+        <v>0</v>
+      </c>
+      <c r="R46" t="n">
         <v>4.3456</v>
       </c>
-      <c r="N46" t="n">
-        <v>0</v>
-      </c>
-      <c r="O46" t="n">
-        <v>0</v>
-      </c>
-      <c r="P46" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q46" t="n">
-        <v>0</v>
-      </c>
-      <c r="R46" t="inlineStr">
+      <c r="S46" t="n">
+        <v>0</v>
+      </c>
+      <c r="T46" t="n">
+        <v>0</v>
+      </c>
+      <c r="U46" t="n">
+        <v>2</v>
+      </c>
+      <c r="V46" t="n">
+        <v>0</v>
+      </c>
+      <c r="W46" t="inlineStr">
         <is>
           <t>07/30/2024</t>
         </is>
       </c>
-      <c r="S46" t="inlineStr">
+      <c r="X46" t="inlineStr">
         <is>
           <t>15:08:41</t>
         </is>
       </c>
-      <c r="T46" t="inlineStr">
+      <c r="Y46" t="inlineStr">
         <is>
           <t>33322222</t>
         </is>
       </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="n">
+        <v>355</v>
+      </c>
+      <c r="C47" t="n">
+        <v>0</v>
+      </c>
+      <c r="D47" t="n">
+        <v>113.1146996035749</v>
+      </c>
+      <c r="E47" t="n">
+        <v>-7.633320652666145</v>
+      </c>
+      <c r="F47" t="n">
+        <v>-14.81854421562475</v>
+      </c>
+      <c r="G47" t="n">
+        <v>0</v>
+      </c>
+      <c r="H47" t="n">
+        <v>0</v>
+      </c>
+      <c r="I47" t="n">
+        <v>0</v>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="K47" t="n">
+        <v>0</v>
+      </c>
+      <c r="L47" t="n">
+        <v>0</v>
+      </c>
+      <c r="M47" t="n">
+        <v>31.0654</v>
+      </c>
+      <c r="N47" t="n">
+        <v>0</v>
+      </c>
+      <c r="O47" t="n">
+        <v>9.933199999999999</v>
+      </c>
+      <c r="P47" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q47" t="n">
+        <v>4.3456</v>
+      </c>
+      <c r="R47" t="n">
+        <v>0</v>
+      </c>
+      <c r="S47" t="n">
+        <v>0</v>
+      </c>
+      <c r="T47" t="n">
+        <v>2</v>
+      </c>
+      <c r="U47" t="n">
+        <v>0</v>
+      </c>
+      <c r="V47" t="inlineStr">
+        <is>
+          <t>07/31/2024</t>
+        </is>
+      </c>
+      <c r="W47" t="inlineStr">
+        <is>
+          <t>08:25:40</t>
+        </is>
+      </c>
+      <c r="X47" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>